<commit_message>
update cable specs and laser warning
</commit_message>
<xml_diff>
--- a/Benchtop-2024(default-version)/parts-list/Benchtop-partslist-latest.xlsx
+++ b/Benchtop-2024(default-version)/parts-list/Benchtop-partslist-latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikita\Documents\GitHub\mesoSPIM-bt-hardware\Benchtop-2024(default-version)\parts-list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55504B1-D03E-4F7E-9F53-ABF755B036F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406209C3-3B8A-4E04-9253-1DAB197978EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="2676" windowWidth="32484" windowHeight="21096" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12492" yWindow="4404" windowWidth="28728" windowHeight="16980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="621">
   <si>
     <t xml:space="preserve">Part # </t>
   </si>
@@ -1787,9 +1787,6 @@
     <t>FOV 25 mm diagonal, programmable rolling shutter, 15MP sensor</t>
   </si>
   <si>
-    <t>Includes switching module between 2 laser ports, controlled by TTL signal. The 405nm is NOT included! A four-laser version is ~35k.</t>
-  </si>
-  <si>
     <t>HW-KIT6</t>
   </si>
   <si>
@@ -1947,6 +1944,30 @@
   </si>
   <si>
     <t>The following specs are suggested for acquisition, not for storage, visualization or image processing</t>
+  </si>
+  <si>
+    <t>The cable MUST be "-EPM". Other similarly looking cables with marking "-RDIO" are NOT suitable.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Warning:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> this is a budget laser, with relatively frequent quality issues. See overview at (https://github.com/mesoSPIM/benchtop-hardware/wiki/Laser-selection). Includes switching module between 2 laser ports, controlled by TTL signal. The 405nm is NOT included! A four-laser version is ~35k.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2722,7 +2743,7 @@
   <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,7 +2851,7 @@
       <c r="E7" s="56"/>
       <c r="F7" s="56"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>161</v>
       </c>
@@ -2851,7 +2872,7 @@
         <v>34</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>566</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -2863,7 +2884,7 @@
     </row>
     <row r="10" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>18</v>
@@ -3001,7 +3022,7 @@
     </row>
     <row r="15" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>18</v>
@@ -3166,13 +3187,13 @@
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D22" s="28">
         <v>0</v>
@@ -3221,10 +3242,10 @@
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>577</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>396</v>
@@ -3242,18 +3263,18 @@
         <v>219</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
@@ -3265,10 +3286,10 @@
         <v>1740</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3295,7 +3316,7 @@
         <v>219</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3383,7 +3404,7 @@
         <v>237</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3410,7 +3431,7 @@
         <v>237</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3496,13 +3517,13 @@
     </row>
     <row r="36" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="82" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>209</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
@@ -3515,7 +3536,7 @@
         <v>10</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="12" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -3527,77 +3548,77 @@
     </row>
     <row r="38" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="86" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E38" s="59"/>
       <c r="F38" s="59"/>
     </row>
     <row r="39" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B39" s="83" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E39" s="85"/>
       <c r="F39" s="85"/>
     </row>
     <row r="40" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="83" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B40" s="83" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E40" s="85"/>
       <c r="F40" s="85"/>
     </row>
     <row r="41" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="83" t="s">
+        <v>611</v>
+      </c>
+      <c r="B41" s="83" t="s">
         <v>612</v>
-      </c>
-      <c r="B41" s="83" t="s">
-        <v>613</v>
       </c>
       <c r="E41" s="85"/>
       <c r="F41" s="85"/>
     </row>
     <row r="42" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="83" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B42" s="83" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E42" s="85"/>
       <c r="F42" s="85"/>
     </row>
     <row r="43" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="83" t="s">
+        <v>606</v>
+      </c>
+      <c r="B43" s="83" t="s">
         <v>607</v>
-      </c>
-      <c r="B43" s="83" t="s">
-        <v>608</v>
       </c>
       <c r="E43" s="85"/>
       <c r="F43" s="85"/>
     </row>
     <row r="44" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
+        <v>616</v>
+      </c>
+      <c r="B44" s="83" t="s">
         <v>617</v>
-      </c>
-      <c r="B44" s="83" t="s">
-        <v>618</v>
       </c>
       <c r="E44" s="85"/>
       <c r="F44" s="85"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>615</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -4452,7 +4473,7 @@
         <v>207</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -4958,13 +4979,13 @@
     </row>
     <row r="93" spans="1:9" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D93" s="4">
         <v>1</v>
@@ -4983,7 +5004,7 @@
         <v>204</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4994,7 +5015,7 @@
         <v>54</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D94" s="3">
         <v>0</v>
@@ -5013,7 +5034,7 @@
         <v>204</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -5569,7 +5590,7 @@
         <v>54</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D122" s="3">
         <v>1</v>
@@ -5732,7 +5753,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>43</v>
@@ -5855,6 +5876,9 @@
       <c r="G133" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="I133" s="3" t="s">
+        <v>619</v>
+      </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
@@ -5912,7 +5936,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>54</v>
@@ -6008,13 +6032,13 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
+        <v>579</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>580</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>581</v>
       </c>
       <c r="D140" s="3">
         <v>1</v>
@@ -6030,7 +6054,7 @@
         <v>44</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -6158,7 +6182,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>54</v>
@@ -6581,13 +6605,13 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>570</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>571</v>
       </c>
       <c r="D168" s="3">
         <v>2</v>
@@ -6600,7 +6624,7 @@
         <v>18</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
@@ -6922,13 +6946,13 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B201" s="3">
         <v>1</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7118,7 +7142,7 @@
     </row>
     <row r="6" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="6" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7151,7 +7175,7 @@
     </row>
     <row r="9" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25"/>
@@ -7712,7 +7736,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>